<commit_message>
Add domentation and setup travis CI
</commit_message>
<xml_diff>
--- a/data/othercase.xlsx
+++ b/data/othercase.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devsisters/Mars/mars-toolbox/JuliaTools/XLSXasJSON/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Company\.julia\packages\XLSXasJSON\it9l8\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCDE48D-7125-C74F-B959-9F577291E418}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2E3BE3-267B-49DE-B60A-FE021A1C6DBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{408D3299-5469-4C4A-A3FE-EC96EFDDFCE6}"/>
+    <workbookView xWindow="11985" yWindow="5955" windowWidth="27645" windowHeight="16935" xr2:uid="{408D3299-5469-4C4A-A3FE-EC96EFDDFCE6}"/>
   </bookViews>
   <sheets>
     <sheet name="compact" sheetId="1" r:id="rId1"/>
-    <sheet name="jsongroup" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -59,78 +58,25 @@
   </si>
   <si>
     <t>MOORE</t>
-  </si>
-  <si>
-    <t>GroupBy{}</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>herbinger</t>
-  </si>
-  <si>
-    <t>marton</t>
-  </si>
-  <si>
-    <t>scropius</t>
-  </si>
-  <si>
-    <t>trump</t>
-  </si>
-  <si>
-    <t>CNN</t>
-  </si>
-  <si>
-    <t>lostark</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Vec[]</t>
-  </si>
-  <si>
-    <t>a;b;c;d</t>
-  </si>
-  <si>
-    <t>d;f;e;g</t>
-  </si>
-  <si>
-    <t>ax</t>
-  </si>
-  <si>
-    <t>az;db</t>
-  </si>
-  <si>
-    <t>ab;bc;cd</t>
-  </si>
-  <si>
-    <t>ff;dd;ee</t>
-  </si>
-  <si>
-    <t>aa;bb;cc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -158,7 +104,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -174,7 +120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -472,13 +418,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD215E79-3421-8D49-A169-EC72AE2AEB01}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A1:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -494,7 +440,7 @@
         <v>1.006</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -502,7 +448,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -510,7 +456,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -518,7 +464,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -526,7 +472,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -534,7 +480,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -542,7 +488,7 @@
         <v>0.42299999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -550,7 +496,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -559,133 +505,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76106006-5F57-8244-B132-8DB839EC9081}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
-        <v>500</v>
-      </c>
-      <c r="D2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>600</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>700</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5">
-        <v>800</v>
-      </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>5000</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>6000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>7000</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove column if key is missing
</commit_message>
<xml_diff>
--- a/data/othercase.xlsx
+++ b/data/othercase.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Company\.julia\packages\XLSXasJSON\it9l8\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devsisters/.julia/packages/XLSXasJSON/aMDJY/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2E3BE3-267B-49DE-B60A-FE021A1C6DBB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD35D7D-BA4A-5E4A-90DA-68F06DBFE2B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="5955" windowWidth="27645" windowHeight="16935" xr2:uid="{408D3299-5469-4C4A-A3FE-EC96EFDDFCE6}"/>
+    <workbookView xWindow="11980" yWindow="5920" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{408D3299-5469-4C4A-A3FE-EC96EFDDFCE6}"/>
   </bookViews>
   <sheets>
     <sheet name="compact" sheetId="1" r:id="rId1"/>
+    <sheet name="missing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -58,6 +59,39 @@
   </si>
   <si>
     <t>MOORE</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>should't read this</t>
+  </si>
+  <si>
+    <t>MICHEAL</t>
+  </si>
+  <si>
+    <t>NULLS</t>
+  </si>
+  <si>
+    <t>Pull</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>AllNull</t>
+  </si>
+  <si>
+    <t>Data.A</t>
+  </si>
+  <si>
+    <t>Data.B</t>
+  </si>
+  <si>
+    <t>issue</t>
   </si>
 </sst>
 </file>
@@ -68,13 +102,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -104,7 +138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -120,7 +154,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -418,13 +452,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD215E79-3421-8D49-A169-EC72AE2AEB01}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -440,7 +474,7 @@
         <v>1.006</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -448,7 +482,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -456,7 +490,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -464,7 +498,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -472,7 +506,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -480,7 +514,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -488,7 +522,7 @@
         <v>0.42299999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -496,7 +530,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -509,4 +543,85 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5652BC7-1071-3C43-A59B-6063908A3B26}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
throw assert for duplicated column name
</commit_message>
<xml_diff>
--- a/data/othercase.xlsx
+++ b/data/othercase.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devsisters/.julia/packages/XLSXasJSON/aMDJY/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devsisters\.julia\dev\XLSXasJSON\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD35D7D-BA4A-5E4A-90DA-68F06DBFE2B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5920" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{408D3299-5469-4C4A-A3FE-EC96EFDDFCE6}"/>
+    <workbookView xWindow="11985" yWindow="5925" windowWidth="27645" windowHeight="16935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="compact" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -92,23 +91,27 @@
   </si>
   <si>
     <t>issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -138,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,16 +452,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD215E79-3421-8D49-A169-EC72AE2AEB01}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -474,7 +477,7 @@
         <v>1.006</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -482,7 +485,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -490,7 +493,7 @@
         <v>0.69899999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -498,7 +501,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -506,7 +509,7 @@
         <v>0.621</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -514,7 +517,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -522,7 +525,7 @@
         <v>0.42299999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -530,7 +533,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -546,16 +549,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5652BC7-1071-3C43-A59B-6063908A3B26}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -569,7 +572,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -580,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -594,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -602,7 +605,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -610,7 +613,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -621,7 +624,13 @@
         <v>50</v>
       </c>
     </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
better structure and testing
</commit_message>
<xml_diff>
--- a/data/othercase.xlsx
+++ b/data/othercase.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="compact" sheetId="1" r:id="rId1"/>
-    <sheet name="missing" sheetId="2" r:id="rId2"/>
+    <sheet name="compactvector" sheetId="3" r:id="rId2"/>
+    <sheet name="missing" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -94,6 +95,62 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vec2[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a;b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b;c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c;d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d;e;f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e;g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f;g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1;5;1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2;5;1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4;3;1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5;1;2;5;1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6;54;5;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vec[Int]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -550,10 +607,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>

</xml_diff>